<commit_message>
Added a copy of the outline with formatted zoop tables
</commit_message>
<xml_diff>
--- a/Zoop_code/Jesse-zoop-analyses/NEWzooptables.xlsx
+++ b/Zoop_code/Jesse-zoop-analyses/NEWzooptables.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\HPG8_backup_8.21.23\Documents\DES docs and forms\NDFA\Manuscript\ND-FASTR\Zoop_code\Jesse-zoop-analyses\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jadams\Documents\DES docs and forms\NDFA\Manuscript\ND-FASTR\Zoop_code\Jesse-zoop-analyses\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F56E82D-CD7A-407E-BC0E-0BC1683BEAC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD34B099-D5B2-46A0-9D51-1B0EA5A821F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1452" yWindow="984" windowWidth="21588" windowHeight="11376" xr2:uid="{AF2E1052-99D4-4F7E-97E0-C211836FA21F}"/>
+    <workbookView xWindow="30570" yWindow="2760" windowWidth="21600" windowHeight="11265" activeTab="1" xr2:uid="{AF2E1052-99D4-4F7E-97E0-C211836FA21F}"/>
   </bookViews>
   <sheets>
     <sheet name="adon.results" sheetId="2" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="108">
   <si>
     <t xml:space="preserve">           F</t>
   </si>
@@ -174,9 +174,6 @@
     <t>Response: log(cpue)</t>
   </si>
   <si>
-    <t xml:space="preserve">                            F Df Df.res    Pr(&gt;F)    </t>
-  </si>
-  <si>
     <t>---</t>
   </si>
   <si>
@@ -364,6 +361,15 @@
   </si>
   <si>
     <t>adon.results &lt;- adonis2(genw2[c(9:70)]~genw2$Region*genw2$SamplePeriod+genw2$Year*genw2$SamplePeriod+genw2$Region*genw2$Year, strata=genw2$StationCode,method=bray,perm=999)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">model4.1_cal &lt;- lmer(log(cpue) ~ Regions2*Year+Year*SamplePeriod+SamplePeriod*Regions2+(1|StationCode),data = zoopNDFA5_calanoid,REML = TRUE) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">model4.1_cyclo &lt;- lmer(log(cpue) ~ Regions2*Year+Year*SamplePeriod+SamplePeriod*Regions2+(1|StationCode),data = zoopNDFA5_cyclopoid,REML = TRUE) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">model4.1_clad &lt;- lmer(log(cpue) ~ Regions2*Year+Year*SamplePeriod+SamplePeriod*Regions2+(1|StationCode),data = zoopNDFA5_cladocera,REML = TRUE) </t>
   </si>
 </sst>
 </file>
@@ -865,7 +871,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C329AF34-7642-45DD-AC80-3E946BA42A8C}">
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
@@ -877,12 +883,12 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -1072,7 +1078,7 @@
   <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+      <selection sqref="A1:F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1082,7 +1088,10 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
+      </c>
+      <c r="B1" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -1099,13 +1108,23 @@
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>42</v>
+      <c r="A5" s="2"/>
+      <c r="B5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" t="s">
+        <v>44</v>
+      </c>
+      <c r="E5" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B6">
         <v>71.600700000000003</v>
@@ -1120,12 +1139,12 @@
         <v>6.9260000000000002E-12</v>
       </c>
       <c r="F6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B7">
         <v>8.2349999999999994</v>
@@ -1140,12 +1159,12 @@
         <v>7.3921000000000004E-3</v>
       </c>
       <c r="F7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B8">
         <v>17.22</v>
@@ -1160,12 +1179,12 @@
         <v>3.6820000000000003E-15</v>
       </c>
       <c r="F8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B9">
         <v>1.7024999999999999</v>
@@ -1182,7 +1201,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B10">
         <v>4.9337</v>
@@ -1197,12 +1216,12 @@
         <v>2.264E-4</v>
       </c>
       <c r="F10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B11">
         <v>4.6285999999999996</v>
@@ -1217,12 +1236,12 @@
         <v>3.4939999999999999E-6</v>
       </c>
       <c r="F11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B12">
         <v>0.49869999999999998</v>
@@ -1239,12 +1258,12 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -1256,8 +1275,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00D368C0-DCD5-45DB-9924-E738418A8B9A}">
   <dimension ref="A1:G29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A19" sqref="A19:B19"/>
+    <sheetView topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1267,12 +1286,12 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B2" t="s">
         <v>34</v>
@@ -1287,7 +1306,7 @@
         <v>30</v>
       </c>
       <c r="F2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G2" t="s">
         <v>28</v>
@@ -1295,7 +1314,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B3" s="5">
         <v>2014</v>
@@ -1318,7 +1337,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B4">
         <v>2015</v>
@@ -1341,7 +1360,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B5" s="5">
         <v>2016</v>
@@ -1364,7 +1383,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B6" s="5">
         <v>2017</v>
@@ -1387,7 +1406,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B7" s="5">
         <v>2018</v>
@@ -1410,7 +1429,7 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B8" s="5">
         <v>2019</v>
@@ -1433,7 +1452,7 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -1892,7 +1911,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27575DC5-E8B3-4281-93C6-BDF935A4CF95}">
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -1903,23 +1922,23 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B3" t="s">
+        <v>100</v>
+      </c>
+      <c r="C3" t="s">
         <v>101</v>
-      </c>
-      <c r="C3" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -2005,20 +2024,20 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="B1" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="C1" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="D1" s="8" t="s">
         <v>85</v>
-      </c>
-      <c r="D1" s="8" t="s">
-        <v>86</v>
       </c>
       <c r="E1" s="8"/>
       <c r="F1" s="8" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G1" s="8"/>
       <c r="H1" s="8"/>
@@ -2028,22 +2047,22 @@
       <c r="B2" s="9"/>
       <c r="C2" s="9"/>
       <c r="D2" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="E2" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="E2" s="7" t="s">
-        <v>88</v>
-      </c>
       <c r="F2" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="G2" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="H2" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="H2" s="7" t="s">
+      <c r="I2" s="7" t="s">
         <v>92</v>
-      </c>
-      <c r="I2" s="7" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -2051,10 +2070,10 @@
         <v>2014</v>
       </c>
       <c r="B3" t="s">
+        <v>79</v>
+      </c>
+      <c r="C3" t="s">
         <v>80</v>
-      </c>
-      <c r="C3" t="s">
-        <v>81</v>
       </c>
       <c r="D3">
         <v>15</v>
@@ -2069,7 +2088,7 @@
         <v>2.6</v>
       </c>
       <c r="I3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -2077,10 +2096,10 @@
         <v>2015</v>
       </c>
       <c r="B4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D4">
         <v>42</v>
@@ -2095,7 +2114,7 @@
         <v>28.4</v>
       </c>
       <c r="I4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -2103,10 +2122,10 @@
         <v>2016</v>
       </c>
       <c r="B5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D5">
         <v>19</v>
@@ -2124,7 +2143,7 @@
         <v>15.8</v>
       </c>
       <c r="I5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -2132,10 +2151,10 @@
         <v>2017</v>
       </c>
       <c r="B6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C6" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D6">
         <v>12</v>
@@ -2153,7 +2172,7 @@
         <v>2.6</v>
       </c>
       <c r="I6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -2161,10 +2180,10 @@
         <v>2018</v>
       </c>
       <c r="B7" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C7" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D7">
         <v>30</v>
@@ -2182,7 +2201,7 @@
         <v>23.6</v>
       </c>
       <c r="I7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -2190,10 +2209,10 @@
         <v>2019</v>
       </c>
       <c r="B8" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C8" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D8">
         <v>26</v>
@@ -2211,7 +2230,7 @@
         <v>32.4</v>
       </c>
       <c r="I8" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
   </sheetData>
@@ -2231,7 +2250,7 @@
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2385,8 +2404,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71C2019C-D9D2-4366-B353-52FA64F823A2}">
   <dimension ref="A1:G29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10:G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2402,12 +2421,12 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B2" t="s">
         <v>34</v>
@@ -2430,7 +2449,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B3" s="5">
         <v>2014</v>
@@ -2453,7 +2472,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B4" s="5">
         <v>2015</v>
@@ -2476,7 +2495,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B5">
         <v>2016</v>
@@ -2499,7 +2518,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B6">
         <v>2017</v>
@@ -2522,7 +2541,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B7" s="5">
         <v>2018</v>
@@ -2545,7 +2564,7 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B8">
         <v>2019</v>
@@ -3033,7 +3052,7 @@
   <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3045,6 +3064,9 @@
       <c r="A1" s="4" t="s">
         <v>39</v>
       </c>
+      <c r="B1" t="s">
+        <v>106</v>
+      </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -3068,7 +3090,7 @@
         <v>24</v>
       </c>
       <c r="D5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E5" t="s">
         <v>20</v>
@@ -3076,7 +3098,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B6">
         <v>34.947600000000001</v>
@@ -3091,12 +3113,12 @@
         <v>9.3340000000000001E-8</v>
       </c>
       <c r="F6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B7">
         <v>5.6532999999999998</v>
@@ -3111,12 +3133,12 @@
         <v>2.2197000000000001E-2</v>
       </c>
       <c r="F7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B8">
         <v>5.5955000000000004</v>
@@ -3131,12 +3153,12 @@
         <v>5.8709999999999999E-5</v>
       </c>
       <c r="F8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B9">
         <v>3.0185</v>
@@ -3151,12 +3173,12 @@
         <v>5.0283000000000001E-2</v>
       </c>
       <c r="F9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B10">
         <v>3.2837999999999998</v>
@@ -3171,12 +3193,12 @@
         <v>6.6109999999999997E-3</v>
       </c>
       <c r="F10" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B11">
         <v>2.5859999999999999</v>
@@ -3191,12 +3213,12 @@
         <v>5.0340000000000003E-3</v>
       </c>
       <c r="F11" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B12">
         <v>0.23130000000000001</v>
@@ -3213,12 +3235,12 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -3230,8 +3252,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0FB4343-2B3A-4546-8374-BA8176CE4411}">
   <dimension ref="A1:K31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A25" sqref="A25:B25"/>
+    <sheetView topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11:G30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3242,18 +3264,18 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B2" t="s">
         <v>34</v>
       </c>
       <c r="C2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D2" t="s">
         <v>26</v>
@@ -3262,7 +3284,7 @@
         <v>30</v>
       </c>
       <c r="F2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G2" t="s">
         <v>28</v>
@@ -3270,7 +3292,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B3" s="5">
         <v>2014</v>
@@ -3293,7 +3315,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B4" s="5">
         <v>2015</v>
@@ -3316,7 +3338,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B5" s="5">
         <v>2016</v>
@@ -3339,7 +3361,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B6" s="5">
         <v>2017</v>
@@ -3362,7 +3384,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B7">
         <v>2018</v>
@@ -3385,7 +3407,7 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B8" s="5">
         <v>2019</v>
@@ -3408,7 +3430,7 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -3882,7 +3904,7 @@
   <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="A5" sqref="A5:XFD5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3892,7 +3914,10 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
+      </c>
+      <c r="B1" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -3909,13 +3934,23 @@
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>42</v>
+      <c r="A5" s="2"/>
+      <c r="B5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" t="s">
+        <v>44</v>
+      </c>
+      <c r="E5" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B6">
         <v>94.525199999999998</v>
@@ -3930,12 +3965,12 @@
         <v>1.356E-6</v>
       </c>
       <c r="F6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B7">
         <v>9.7042999999999999</v>
@@ -3950,12 +3985,12 @@
         <v>1.2333E-2</v>
       </c>
       <c r="F7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B8">
         <v>2.9376000000000002</v>
@@ -3970,12 +4005,12 @@
         <v>1.3072E-2</v>
       </c>
       <c r="F8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B9">
         <v>3.2650000000000001</v>
@@ -3990,12 +4025,12 @@
         <v>3.9437E-2</v>
       </c>
       <c r="F9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B10">
         <v>6.6181000000000001</v>
@@ -4010,12 +4045,12 @@
         <v>6.8959999999999997E-6</v>
       </c>
       <c r="F10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B11">
         <v>1.6382000000000001</v>
@@ -4030,12 +4065,12 @@
         <v>9.4579999999999997E-2</v>
       </c>
       <c r="F11" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B12">
         <v>6.2704000000000004</v>
@@ -4050,17 +4085,17 @@
         <v>2.1250000000000002E-3</v>
       </c>
       <c r="F12" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -4073,7 +4108,7 @@
   <dimension ref="A1:G23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+      <selection activeCell="A16" sqref="A16:G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4086,27 +4121,27 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B2" t="s">
         <v>34</v>
       </c>
       <c r="C2" t="s">
+        <v>64</v>
+      </c>
+      <c r="D2" t="s">
         <v>65</v>
-      </c>
-      <c r="D2" t="s">
-        <v>66</v>
       </c>
       <c r="E2" t="s">
         <v>30</v>
       </c>
       <c r="F2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G2" t="s">
         <v>28</v>
@@ -4114,7 +4149,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B3" s="5">
         <v>2014</v>
@@ -4137,7 +4172,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B4" s="5">
         <v>2015</v>
@@ -4160,7 +4195,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B5">
         <v>2016</v>
@@ -4183,7 +4218,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B6">
         <v>2017</v>
@@ -4206,7 +4241,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B7" s="5">
         <v>2018</v>
@@ -4229,7 +4264,7 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B8" s="5">
         <v>2019</v>
@@ -4252,27 +4287,27 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B11" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C11" t="s">
+        <v>64</v>
+      </c>
+      <c r="D11" t="s">
         <v>65</v>
-      </c>
-      <c r="D11" t="s">
-        <v>66</v>
       </c>
       <c r="E11" t="s">
         <v>30</v>
       </c>
       <c r="F11" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G11" t="s">
         <v>28</v>
@@ -4280,10 +4315,10 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C12">
         <v>2.5899770000000002</v>
@@ -4303,10 +4338,10 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C13">
         <v>3.4945710000000001</v>
@@ -4326,10 +4361,10 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B14" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C14">
         <v>2.2188970000000001</v>
@@ -4349,7 +4384,7 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
changed the look of plot Upstream and Downstream Total BV by ActionPhase for each year
</commit_message>
<xml_diff>
--- a/Zoop_code/Jesse-zoop-analyses/NEWzooptables.xlsx
+++ b/Zoop_code/Jesse-zoop-analyses/NEWzooptables.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jadams\Documents\DES docs and forms\NDFA\Manuscript\ND-FASTR\Zoop_code\Jesse-zoop-analyses\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD34B099-D5B2-46A0-9D51-1B0EA5A821F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5D36022-9454-4B02-A094-2A8C2F9586DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30570" yWindow="2760" windowWidth="21600" windowHeight="11265" activeTab="1" xr2:uid="{AF2E1052-99D4-4F7E-97E0-C211836FA21F}"/>
+    <workbookView xWindow="0" yWindow="30" windowWidth="19200" windowHeight="11510" xr2:uid="{AF2E1052-99D4-4F7E-97E0-C211836FA21F}"/>
   </bookViews>
   <sheets>
     <sheet name="adon.results" sheetId="2" r:id="rId1"/>
@@ -21,8 +21,8 @@
     <sheet name="ANOVA_cyclo" sheetId="6" r:id="rId6"/>
     <sheet name="posthoc_cyclo" sheetId="9" r:id="rId7"/>
     <sheet name="ANOVA_cal" sheetId="7" r:id="rId8"/>
-    <sheet name="posthoc_cal" sheetId="10" r:id="rId9"/>
-    <sheet name="ANOVA_clad" sheetId="8" r:id="rId10"/>
+    <sheet name="ANOVA_clad" sheetId="8" r:id="rId9"/>
+    <sheet name="posthoc_cal" sheetId="10" r:id="rId10"/>
     <sheet name="posthoc_clad" sheetId="13" r:id="rId11"/>
   </sheets>
   <calcPr calcId="191029"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="109">
   <si>
     <t xml:space="preserve">           F</t>
   </si>
@@ -370,12 +370,18 @@
   </si>
   <si>
     <t xml:space="preserve">model4.1_clad &lt;- lmer(log(cpue) ~ Regions2*Year+Year*SamplePeriod+SamplePeriod*Regions2+(1|StationCode),data = zoopNDFA5_cladocera,REML = TRUE) </t>
+  </si>
+  <si>
+    <t>&lt; 0.001</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="172" formatCode="0.000"/>
+  </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -429,7 +435,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -444,7 +450,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -453,6 +458,20 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -871,8 +890,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C329AF34-7642-45DD-AC80-3E946BA42A8C}">
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4:E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -915,13 +934,13 @@
       <c r="B4">
         <v>1</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="9">
         <v>12.354916390297401</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="9">
         <v>9.3421638659728801E-2</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="9">
         <v>45.270796632738502</v>
       </c>
       <c r="F4">
@@ -935,13 +954,13 @@
       <c r="B5">
         <v>2</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="9">
         <v>2.3908725709781602</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="9">
         <v>1.80785710199373E-2</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="9">
         <v>4.3803091221461301</v>
       </c>
       <c r="F5">
@@ -955,13 +974,13 @@
       <c r="B6">
         <v>1</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="9">
         <v>10.994764995959001</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="9">
         <v>8.3136860675784199E-2</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="9">
         <v>40.2869395820194</v>
       </c>
       <c r="F6">
@@ -975,13 +994,13 @@
       <c r="B7">
         <v>2</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="9">
         <v>1.8486074702172</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="9">
         <v>1.39782361653157E-2</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="9">
         <v>3.3868271623305302</v>
       </c>
       <c r="F7">
@@ -995,13 +1014,13 @@
       <c r="B8">
         <v>2</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="9">
         <v>1.0243274345248901</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="9">
         <v>7.7454467868825197E-3</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="9">
         <v>1.8766666446293401</v>
       </c>
       <c r="F8">
@@ -1015,13 +1034,13 @@
       <c r="B9">
         <v>1</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="9">
         <v>3.2040963868979002</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="9">
         <v>2.4227758847707798E-2</v>
       </c>
-      <c r="E9">
+      <c r="E9" s="9">
         <v>11.7404271579579</v>
       </c>
       <c r="F9">
@@ -1035,13 +1054,13 @@
       <c r="B10">
         <v>368</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="9">
         <v>100.431394404521</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="9">
         <v>0.75941148784464296</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E10" s="9" t="s">
         <v>11</v>
       </c>
       <c r="F10" t="s">
@@ -1055,13 +1074,13 @@
       <c r="B11">
         <v>377</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="9">
         <v>132.24897965339599</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="9">
         <v>1</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E11" s="9" t="s">
         <v>11</v>
       </c>
       <c r="F11" t="s">
@@ -1074,199 +1093,466 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{581420B1-334D-4801-9E0F-AB9FD07C8D35}">
-  <dimension ref="A1:F14"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{608A0460-4DAE-480E-BE49-2A986203EA97}">
+  <dimension ref="A1:G23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:F14"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18:G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.42578125" customWidth="1"/>
+    <col min="1" max="1" width="22.5703125" customWidth="1"/>
+    <col min="2" max="2" width="16.28515625" customWidth="1"/>
+    <col min="12" max="12" width="22.42578125" customWidth="1"/>
+    <col min="13" max="13" width="14.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="B1" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="1"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="2"/>
-      <c r="B5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C5" t="s">
-        <v>24</v>
-      </c>
-      <c r="D5" t="s">
-        <v>44</v>
-      </c>
-      <c r="E5" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>45</v>
+        <v>67</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C2" t="s">
+        <v>64</v>
+      </c>
+      <c r="D2" t="s">
+        <v>65</v>
+      </c>
+      <c r="E2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F2" t="s">
+        <v>66</v>
+      </c>
+      <c r="G2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="B3" s="5">
+        <v>2014</v>
+      </c>
+      <c r="C3" s="9">
+        <v>3.6538819999999999</v>
+      </c>
+      <c r="D3" s="9">
+        <v>1.0993759999999999</v>
+      </c>
+      <c r="E3" s="9">
+        <v>8.5289640000000002</v>
+      </c>
+      <c r="F3" s="9">
+        <v>3.3235980000000001</v>
+      </c>
+      <c r="G3" s="9">
+        <v>9.5791999999999995E-3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="B4" s="5">
+        <v>2015</v>
+      </c>
+      <c r="C4" s="9">
+        <v>3.6646580000000002</v>
+      </c>
+      <c r="D4" s="9">
+        <v>1.0904290000000001</v>
+      </c>
+      <c r="E4" s="9">
+        <v>8.2551600000000001</v>
+      </c>
+      <c r="F4" s="9">
+        <v>3.3607480000000001</v>
+      </c>
+      <c r="G4" s="9">
+        <v>9.4801E-3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>61</v>
+      </c>
+      <c r="B5">
+        <v>2016</v>
+      </c>
+      <c r="C5" s="9">
+        <v>2.3328340000000001</v>
+      </c>
+      <c r="D5" s="9">
+        <v>1.1052040000000001</v>
+      </c>
+      <c r="E5" s="9">
+        <v>8.7099390000000003</v>
+      </c>
+      <c r="F5" s="9">
+        <v>2.110773</v>
+      </c>
+      <c r="G5" s="9">
+        <v>6.5000500000000003E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>61</v>
       </c>
       <c r="B6">
-        <v>71.600700000000003</v>
-      </c>
-      <c r="C6">
-        <v>1</v>
-      </c>
-      <c r="D6">
-        <v>61.19</v>
-      </c>
-      <c r="E6" s="6">
-        <v>6.9260000000000002E-12</v>
-      </c>
-      <c r="F6" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="B7">
-        <v>8.2349999999999994</v>
-      </c>
-      <c r="C7">
-        <v>1</v>
-      </c>
-      <c r="D7">
-        <v>30.54</v>
-      </c>
-      <c r="E7">
-        <v>7.3921000000000004E-3</v>
-      </c>
-      <c r="F7" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="B8">
-        <v>17.22</v>
-      </c>
-      <c r="C8">
-        <v>5</v>
-      </c>
-      <c r="D8">
-        <v>333.48</v>
-      </c>
-      <c r="E8" s="6">
-        <v>3.6820000000000003E-15</v>
-      </c>
-      <c r="F8" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="B9">
-        <v>1.7024999999999999</v>
-      </c>
-      <c r="C9">
-        <v>2</v>
-      </c>
-      <c r="D9">
-        <v>333.1</v>
-      </c>
-      <c r="E9">
-        <v>0.18380650000000001</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="B10">
-        <v>4.9337</v>
-      </c>
-      <c r="C10">
-        <v>5</v>
-      </c>
-      <c r="D10">
-        <v>333.51</v>
-      </c>
-      <c r="E10">
-        <v>2.264E-4</v>
-      </c>
-      <c r="F10" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="B11">
-        <v>4.6285999999999996</v>
-      </c>
-      <c r="C11">
-        <v>10</v>
-      </c>
-      <c r="D11">
-        <v>333.38</v>
-      </c>
-      <c r="E11" s="6">
-        <v>3.4939999999999999E-6</v>
+        <v>2017</v>
+      </c>
+      <c r="C6" s="9">
+        <v>1.2274240000000001</v>
+      </c>
+      <c r="D6" s="9">
+        <v>1.102522</v>
+      </c>
+      <c r="E6" s="9">
+        <v>8.6264389999999995</v>
+      </c>
+      <c r="F6" s="9">
+        <v>1.1132880000000001</v>
+      </c>
+      <c r="G6" s="9">
+        <v>0.29564259999999998</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="B7" s="5">
+        <v>2018</v>
+      </c>
+      <c r="C7" s="9">
+        <v>3.1665100000000002</v>
+      </c>
+      <c r="D7" s="9">
+        <v>1.0763849999999999</v>
+      </c>
+      <c r="E7" s="9">
+        <v>7.8378379999999996</v>
+      </c>
+      <c r="F7" s="9">
+        <v>2.9418000000000002</v>
+      </c>
+      <c r="G7" s="9">
+        <v>1.90828E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="B8" s="5">
+        <v>2019</v>
+      </c>
+      <c r="C8" s="9">
+        <v>2.5615809999999999</v>
+      </c>
+      <c r="D8" s="9">
+        <v>1.099496</v>
+      </c>
+      <c r="E8" s="9">
+        <v>8.532724</v>
+      </c>
+      <c r="F8" s="9">
+        <v>2.329777</v>
+      </c>
+      <c r="G8" s="9">
+        <v>4.6254000000000003E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>58</v>
+      </c>
+      <c r="B11" t="s">
+        <v>68</v>
+      </c>
+      <c r="C11" t="s">
+        <v>64</v>
+      </c>
+      <c r="D11" t="s">
+        <v>65</v>
+      </c>
+      <c r="E11" t="s">
+        <v>30</v>
       </c>
       <c r="F11" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="B12">
-        <v>0.49869999999999998</v>
-      </c>
-      <c r="C12">
-        <v>2</v>
-      </c>
-      <c r="D12">
-        <v>333.23</v>
-      </c>
-      <c r="E12">
-        <v>0.60778109999999996</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
-        <v>43</v>
+        <v>66</v>
+      </c>
+      <c r="G11" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="C12" s="9">
+        <v>2.5899770000000002</v>
+      </c>
+      <c r="D12" s="9">
+        <v>1.0633900000000001</v>
+      </c>
+      <c r="E12" s="9">
+        <v>7.4673660000000002</v>
+      </c>
+      <c r="F12" s="9">
+        <v>2.435584</v>
+      </c>
+      <c r="G12" s="9">
+        <v>4.2934E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="C13" s="9">
+        <v>3.4945710000000001</v>
+      </c>
+      <c r="D13" s="9">
+        <v>1.0718620000000001</v>
+      </c>
+      <c r="E13" s="9">
+        <v>7.7080200000000003</v>
+      </c>
+      <c r="F13" s="9">
+        <v>3.2602799999999998</v>
+      </c>
+      <c r="G13" s="9">
+        <v>1.2124299999999999E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>61</v>
+      </c>
+      <c r="B14" t="s">
+        <v>71</v>
+      </c>
+      <c r="C14" s="9">
+        <v>2.2188970000000001</v>
+      </c>
+      <c r="D14" s="9">
+        <v>1.064174</v>
+      </c>
+      <c r="E14" s="9">
+        <v>7.4889239999999999</v>
+      </c>
+      <c r="F14" s="9">
+        <v>2.0850870000000001</v>
+      </c>
+      <c r="G14" s="9">
+        <v>7.2922299999999995E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>33</v>
+      </c>
+      <c r="B17" t="s">
+        <v>29</v>
+      </c>
+      <c r="C17" t="s">
+        <v>25</v>
+      </c>
+      <c r="D17" t="s">
+        <v>26</v>
+      </c>
+      <c r="E17" t="s">
+        <v>30</v>
+      </c>
+      <c r="F17" t="s">
+        <v>27</v>
+      </c>
+      <c r="G17" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>35</v>
+      </c>
+      <c r="B18" t="s">
+        <v>31</v>
+      </c>
+      <c r="C18" s="9">
+        <v>-0.1036161</v>
+      </c>
+      <c r="D18" s="9">
+        <v>0.26980330000000002</v>
+      </c>
+      <c r="E18" s="9">
+        <v>329.00450000000001</v>
+      </c>
+      <c r="F18" s="9">
+        <v>-0.38404300000000002</v>
+      </c>
+      <c r="G18" s="9">
+        <v>0.97332129999999994</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>36</v>
+      </c>
+      <c r="B19" t="s">
+        <v>31</v>
+      </c>
+      <c r="C19" s="9">
+        <v>0.58866350000000001</v>
+      </c>
+      <c r="D19" s="9">
+        <v>0.25318770000000002</v>
+      </c>
+      <c r="E19" s="9">
+        <v>329.00630000000001</v>
+      </c>
+      <c r="F19" s="9">
+        <v>2.3250082999999999</v>
+      </c>
+      <c r="G19" s="9">
+        <v>6.07643E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C20" s="9">
+        <v>0.69227959999999999</v>
+      </c>
+      <c r="D20" s="9">
+        <v>0.27322590000000002</v>
+      </c>
+      <c r="E20" s="9">
+        <v>329.00819999999999</v>
+      </c>
+      <c r="F20" s="9">
+        <v>2.5337261</v>
+      </c>
+      <c r="G20" s="9">
+        <v>3.4835699999999997E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C21" s="9">
+        <v>0.80097830000000003</v>
+      </c>
+      <c r="D21" s="9">
+        <v>0.2534402</v>
+      </c>
+      <c r="E21" s="9">
+        <v>329.03910000000002</v>
+      </c>
+      <c r="F21" s="9">
+        <v>3.1604231999999999</v>
+      </c>
+      <c r="G21" s="9">
+        <v>5.1564000000000002E-3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>36</v>
+      </c>
+      <c r="B22" t="s">
+        <v>32</v>
+      </c>
+      <c r="C22" s="9">
+        <v>0.21758350000000001</v>
+      </c>
+      <c r="D22" s="9">
+        <v>0.2365738</v>
+      </c>
+      <c r="E22" s="9">
+        <v>329.125</v>
+      </c>
+      <c r="F22" s="9">
+        <v>0.91972759999999998</v>
+      </c>
+      <c r="G22" s="9">
+        <v>0.7358711</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>37</v>
+      </c>
+      <c r="B23" t="s">
+        <v>32</v>
+      </c>
+      <c r="C23" s="9">
+        <v>-0.58339479999999999</v>
+      </c>
+      <c r="D23" s="9">
+        <v>0.263714</v>
+      </c>
+      <c r="E23" s="9">
+        <v>329.24059999999997</v>
+      </c>
+      <c r="F23" s="9">
+        <v>-2.2122255000000002</v>
+      </c>
+      <c r="G23" s="9">
+        <v>8.0641000000000004E-2</v>
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="G3:G8">
+    <cfRule type="cellIs" dxfId="4" priority="3" operator="lessThan">
+      <formula>0.06</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G12:G14">
+    <cfRule type="cellIs" dxfId="3" priority="2" operator="lessThan">
+      <formula>0.06</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G18:G23">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="lessThan">
+      <formula>0.06</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1276,7 +1562,7 @@
   <dimension ref="A1:G29"/>
   <sheetViews>
     <sheetView topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+      <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1319,19 +1605,19 @@
       <c r="B3" s="5">
         <v>2014</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="9">
         <v>-1.3403967999999999</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="9">
         <v>0.49306879999999997</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="9">
         <v>22.931819999999998</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="9">
         <v>-2.7184780000000002</v>
       </c>
-      <c r="G3">
+      <c r="G3" s="9">
         <v>1.2272699999999999E-2</v>
       </c>
     </row>
@@ -1342,19 +1628,19 @@
       <c r="B4">
         <v>2015</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="9">
         <v>-0.51655569999999995</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="9">
         <v>0.46914739999999999</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="9">
         <v>18.886389999999999</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="9">
         <v>-1.1010519999999999</v>
       </c>
-      <c r="G4">
+      <c r="G4" s="9">
         <v>0.2847094</v>
       </c>
     </row>
@@ -1365,19 +1651,19 @@
       <c r="B5" s="5">
         <v>2016</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="9">
         <v>-1.5933208000000001</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="9">
         <v>0.4871065</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="9">
         <v>21.809270000000001</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="9">
         <v>-3.270991</v>
       </c>
-      <c r="G5">
+      <c r="G5" s="9">
         <v>3.5222999999999999E-3</v>
       </c>
     </row>
@@ -1388,19 +1674,19 @@
       <c r="B6" s="5">
         <v>2017</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="9">
         <v>-2.4586942999999999</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="9">
         <v>0.4903805</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="9">
         <v>22.420089999999998</v>
       </c>
-      <c r="F6">
+      <c r="F6" s="9">
         <v>-5.0138499999999997</v>
       </c>
-      <c r="G6">
+      <c r="G6" s="9">
         <v>4.8300000000000002E-5</v>
       </c>
     </row>
@@ -1411,19 +1697,19 @@
       <c r="B7" s="5">
         <v>2018</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="9">
         <v>-1.09389</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="9">
         <v>0.43597069999999999</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="9">
         <v>14.07667</v>
       </c>
-      <c r="F7">
+      <c r="F7" s="9">
         <v>-2.5090910000000002</v>
       </c>
-      <c r="G7">
+      <c r="G7" s="9">
         <v>2.49448E-2</v>
       </c>
     </row>
@@ -1434,19 +1720,19 @@
       <c r="B8" s="5">
         <v>2019</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="9">
         <v>-2.3282832</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="9">
         <v>0.48735410000000001</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="9">
         <v>21.92191</v>
       </c>
-      <c r="F8">
+      <c r="F8" s="9">
         <v>-4.7773950000000003</v>
       </c>
-      <c r="G8">
+      <c r="G8" s="9">
         <v>9.1199999999999994E-5</v>
       </c>
     </row>
@@ -1485,19 +1771,19 @@
       <c r="B12">
         <v>2014</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="9">
         <v>-0.37679430000000003</v>
       </c>
-      <c r="D12">
+      <c r="D12" s="9">
         <v>0.52737619999999996</v>
       </c>
-      <c r="E12">
+      <c r="E12" s="9">
         <v>333.06450000000001</v>
       </c>
-      <c r="F12">
+      <c r="F12" s="9">
         <v>-0.71446969999999999</v>
       </c>
-      <c r="G12">
+      <c r="G12" s="9">
         <v>0.85565809999999998</v>
       </c>
     </row>
@@ -1508,19 +1794,19 @@
       <c r="B13">
         <v>2014</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="9">
         <v>-0.70233049999999997</v>
       </c>
-      <c r="D13">
+      <c r="D13" s="9">
         <v>0.3975996</v>
       </c>
-      <c r="E13">
+      <c r="E13" s="9">
         <v>333.12790000000001</v>
       </c>
-      <c r="F13">
+      <c r="F13" s="9">
         <v>-1.7664268000000001</v>
       </c>
-      <c r="G13">
+      <c r="G13" s="9">
         <v>0.21683459999999999</v>
       </c>
     </row>
@@ -1531,19 +1817,19 @@
       <c r="B14">
         <v>2014</v>
       </c>
-      <c r="C14">
+      <c r="C14" s="9">
         <v>-0.3255362</v>
       </c>
-      <c r="D14">
+      <c r="D14" s="9">
         <v>0.48398639999999998</v>
       </c>
-      <c r="E14">
+      <c r="E14" s="9">
         <v>333.00920000000002</v>
       </c>
-      <c r="F14">
+      <c r="F14" s="9">
         <v>-0.67261439999999995</v>
       </c>
-      <c r="G14">
+      <c r="G14" s="9">
         <v>0.87624020000000002</v>
       </c>
     </row>
@@ -1554,19 +1840,19 @@
       <c r="B15" s="5">
         <v>2015</v>
       </c>
-      <c r="C15">
+      <c r="C15" s="9">
         <v>-1.3113797</v>
       </c>
-      <c r="D15">
+      <c r="D15" s="9">
         <v>0.40038469999999998</v>
       </c>
-      <c r="E15">
+      <c r="E15" s="9">
         <v>333.21570000000003</v>
       </c>
-      <c r="F15">
+      <c r="F15" s="9">
         <v>-3.2752992999999999</v>
       </c>
-      <c r="G15">
+      <c r="G15" s="9">
         <v>3.4952999999999998E-3</v>
       </c>
     </row>
@@ -1577,19 +1863,19 @@
       <c r="B16" s="5">
         <v>2015</v>
       </c>
-      <c r="C16">
+      <c r="C16" s="9">
         <v>-1.1909498999999999</v>
       </c>
-      <c r="D16">
+      <c r="D16" s="9">
         <v>0.40045999999999998</v>
       </c>
-      <c r="E16">
+      <c r="E16" s="9">
         <v>333.41399999999999</v>
       </c>
-      <c r="F16">
+      <c r="F16" s="9">
         <v>-2.9739545999999999</v>
       </c>
-      <c r="G16">
+      <c r="G16" s="9">
         <v>9.4325999999999993E-3</v>
       </c>
     </row>
@@ -1600,19 +1886,19 @@
       <c r="B17">
         <v>2015</v>
       </c>
-      <c r="C17">
+      <c r="C17" s="9">
         <v>0.1204298</v>
       </c>
-      <c r="D17">
+      <c r="D17" s="9">
         <v>0.37739279999999997</v>
       </c>
-      <c r="E17">
+      <c r="E17" s="9">
         <v>333.07459999999998</v>
       </c>
-      <c r="F17">
+      <c r="F17" s="9">
         <v>0.31911</v>
       </c>
-      <c r="G17">
+      <c r="G17" s="9">
         <v>0.98434560000000004</v>
       </c>
     </row>
@@ -1623,19 +1909,19 @@
       <c r="B18">
         <v>2016</v>
       </c>
-      <c r="C18">
+      <c r="C18" s="9">
         <v>1.2143454</v>
       </c>
-      <c r="D18">
+      <c r="D18" s="9">
         <v>0.53339930000000002</v>
       </c>
-      <c r="E18">
+      <c r="E18" s="9">
         <v>333.34120000000001</v>
       </c>
-      <c r="F18">
+      <c r="F18" s="9">
         <v>2.2766161</v>
       </c>
-      <c r="G18">
+      <c r="G18" s="9">
         <v>6.8692199999999995E-2</v>
       </c>
     </row>
@@ -1646,19 +1932,19 @@
       <c r="B19" s="5">
         <v>2016</v>
       </c>
-      <c r="C19">
+      <c r="C19" s="9">
         <v>2.0162083000000002</v>
       </c>
-      <c r="D19">
+      <c r="D19" s="9">
         <v>0.39862069999999999</v>
       </c>
-      <c r="E19">
+      <c r="E19" s="9">
         <v>333.7373</v>
       </c>
-      <c r="F19">
+      <c r="F19" s="9">
         <v>5.0579624000000001</v>
       </c>
-      <c r="G19">
+      <c r="G19" s="9">
         <v>2.0999999999999998E-6</v>
       </c>
     </row>
@@ -1669,19 +1955,19 @@
       <c r="B20">
         <v>2016</v>
       </c>
-      <c r="C20">
+      <c r="C20" s="9">
         <v>0.80186290000000005</v>
       </c>
-      <c r="D20">
+      <c r="D20" s="9">
         <v>0.47890050000000001</v>
       </c>
-      <c r="E20">
+      <c r="E20" s="9">
         <v>333.322</v>
       </c>
-      <c r="F20">
+      <c r="F20" s="9">
         <v>1.6743832000000001</v>
       </c>
-      <c r="G20">
+      <c r="G20" s="9">
         <v>0.25876589999999999</v>
       </c>
     </row>
@@ -1692,19 +1978,19 @@
       <c r="B21">
         <v>2017</v>
       </c>
-      <c r="C21">
+      <c r="C21" s="9">
         <v>-0.50571880000000002</v>
       </c>
-      <c r="D21">
+      <c r="D21" s="9">
         <v>0.38441959999999997</v>
       </c>
-      <c r="E21">
+      <c r="E21" s="9">
         <v>333.00220000000002</v>
       </c>
-      <c r="F21">
+      <c r="F21" s="9">
         <v>-1.3155387000000001</v>
       </c>
-      <c r="G21">
+      <c r="G21" s="9">
         <v>0.46704980000000001</v>
       </c>
     </row>
@@ -1715,19 +2001,19 @@
       <c r="B22">
         <v>2017</v>
       </c>
-      <c r="C22">
+      <c r="C22" s="9">
         <v>-5.90252E-2</v>
       </c>
-      <c r="D22">
+      <c r="D22" s="9">
         <v>0.51476670000000002</v>
       </c>
-      <c r="E22">
+      <c r="E22" s="9">
         <v>334.90280000000001</v>
       </c>
-      <c r="F22">
+      <c r="F22" s="9">
         <v>-0.1146639</v>
       </c>
-      <c r="G22">
+      <c r="G22" s="9">
         <v>0.99924100000000005</v>
       </c>
     </row>
@@ -1738,19 +2024,19 @@
       <c r="B23">
         <v>2017</v>
       </c>
-      <c r="C23">
+      <c r="C23" s="9">
         <v>0.44669370000000003</v>
       </c>
-      <c r="D23">
+      <c r="D23" s="9">
         <v>0.54266250000000005</v>
       </c>
-      <c r="E23">
+      <c r="E23" s="9">
         <v>334.71179999999998</v>
       </c>
-      <c r="F23">
+      <c r="F23" s="9">
         <v>0.82315199999999999</v>
       </c>
-      <c r="G23">
+      <c r="G23" s="9">
         <v>0.79567149999999998</v>
       </c>
     </row>
@@ -1761,19 +2047,19 @@
       <c r="B24">
         <v>2018</v>
       </c>
-      <c r="C24">
+      <c r="C24" s="9">
         <v>-0.6907063</v>
       </c>
-      <c r="D24">
+      <c r="D24" s="9">
         <v>0.33858519999999998</v>
       </c>
-      <c r="E24">
+      <c r="E24" s="9">
         <v>333.02719999999999</v>
       </c>
-      <c r="F24">
+      <c r="F24" s="9">
         <v>-2.0399777000000001</v>
       </c>
-      <c r="G24">
+      <c r="G24" s="9">
         <v>0.1211708</v>
       </c>
     </row>
@@ -1784,19 +2070,19 @@
       <c r="B25">
         <v>2018</v>
       </c>
-      <c r="C25">
+      <c r="C25" s="9">
         <v>-0.46507280000000001</v>
       </c>
-      <c r="D25">
+      <c r="D25" s="9">
         <v>0.3164284</v>
       </c>
-      <c r="E25">
+      <c r="E25" s="9">
         <v>333.3843</v>
       </c>
-      <c r="F25">
+      <c r="F25" s="9">
         <v>-1.4697566</v>
       </c>
-      <c r="G25">
+      <c r="G25" s="9">
         <v>0.36963089999999998</v>
       </c>
     </row>
@@ -1807,19 +2093,19 @@
       <c r="B26">
         <v>2018</v>
       </c>
-      <c r="C26">
+      <c r="C26" s="9">
         <v>0.22563349999999999</v>
       </c>
-      <c r="D26">
+      <c r="D26" s="9">
         <v>0.34345920000000002</v>
       </c>
-      <c r="E26">
+      <c r="E26" s="9">
         <v>333.17689999999999</v>
       </c>
-      <c r="F26">
+      <c r="F26" s="9">
         <v>0.65694410000000003</v>
       </c>
-      <c r="G26">
+      <c r="G26" s="9">
         <v>0.8835501</v>
       </c>
     </row>
@@ -1830,19 +2116,19 @@
       <c r="B27">
         <v>2019</v>
       </c>
-      <c r="C27">
+      <c r="C27" s="9">
         <v>0.26053029999999999</v>
       </c>
-      <c r="D27">
+      <c r="D27" s="9">
         <v>0.42772579999999999</v>
       </c>
-      <c r="E27">
+      <c r="E27" s="9">
         <v>333.05329999999998</v>
       </c>
-      <c r="F27">
+      <c r="F27" s="9">
         <v>0.60910589999999998</v>
       </c>
-      <c r="G27">
+      <c r="G27" s="9">
         <v>0.90447420000000001</v>
       </c>
     </row>
@@ -1853,19 +2139,19 @@
       <c r="B28">
         <v>2019</v>
       </c>
-      <c r="C28">
+      <c r="C28" s="9">
         <v>0.86908940000000001</v>
       </c>
-      <c r="D28">
+      <c r="D28" s="9">
         <v>0.42766729999999997</v>
       </c>
-      <c r="E28">
+      <c r="E28" s="9">
         <v>333.05579999999998</v>
       </c>
-      <c r="F28">
+      <c r="F28" s="9">
         <v>2.0321625000000001</v>
       </c>
-      <c r="G28">
+      <c r="G28" s="9">
         <v>0.1233413</v>
       </c>
     </row>
@@ -1876,19 +2162,19 @@
       <c r="B29">
         <v>2019</v>
       </c>
-      <c r="C29">
+      <c r="C29" s="9">
         <v>0.60855910000000002</v>
       </c>
-      <c r="D29">
+      <c r="D29" s="9">
         <v>0.4210275</v>
       </c>
-      <c r="E29">
+      <c r="E29" s="9">
         <v>333.0027</v>
       </c>
-      <c r="F29">
+      <c r="F29" s="9">
         <v>1.4454142000000001</v>
       </c>
-      <c r="G29">
+      <c r="G29" s="9">
         <v>0.38431739999999998</v>
       </c>
     </row>
@@ -1911,7 +2197,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27575DC5-E8B3-4281-93C6-BDF935A4CF95}">
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -2023,45 +2309,45 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8" t="s">
+      <c r="E1" s="7"/>
+      <c r="F1" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
     </row>
     <row r="2" spans="1:9" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="9"/>
-      <c r="B2" s="9"/>
-      <c r="C2" s="9"/>
-      <c r="D2" s="7" t="s">
+      <c r="A2" s="8"/>
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="6" t="s">
         <v>86</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="E2" s="6" t="s">
         <v>87</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="F2" s="6" t="s">
         <v>89</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="G2" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="H2" s="7" t="s">
+      <c r="H2" s="6" t="s">
         <v>91</v>
       </c>
-      <c r="I2" s="7" t="s">
+      <c r="I2" s="6" t="s">
         <v>92</v>
       </c>
     </row>
@@ -2250,15 +2536,16 @@
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="B2" sqref="B2:B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="3.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -2276,121 +2563,121 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="12">
         <v>411.5105456</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="13">
         <v>1</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="14">
         <v>52.147689999999997</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="14">
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="12">
         <v>7.3091530000000002</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="13">
         <v>1</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="14">
         <v>29.79917</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="14">
         <v>1.12207E-2</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="A4" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="12">
         <v>5.4255161000000003</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="13">
         <v>5</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="14">
         <v>339.36282</v>
       </c>
-      <c r="E4">
-        <v>8.1199999999999995E-5</v>
+      <c r="E4" s="14" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="A5" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="12">
         <v>0.56769340000000001</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="13">
         <v>2</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="14">
         <v>339.02843000000001</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="14">
         <v>0.56736929999999997</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="A6" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="12">
         <v>6.7527461000000004</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="13">
         <v>5</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="14">
         <v>339.46836000000002</v>
       </c>
-      <c r="E6">
-        <v>5.1000000000000003E-6</v>
+      <c r="E6" s="14" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="A7" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="12">
         <v>1.8650837</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="13">
         <v>10</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="14">
         <v>339.39407</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="14">
         <v>4.9051900000000002E-2</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="A8" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="12">
         <v>2.7466134000000002</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="13">
         <v>2</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="14">
         <v>339.17196999999999</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="14">
         <v>6.5571900000000002E-2</v>
       </c>
     </row>
@@ -2404,19 +2691,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71C2019C-D9D2-4366-B353-52FA64F823A2}">
   <dimension ref="A1:G29"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:G29"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3:G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="24.7109375" customWidth="1"/>
     <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -2454,19 +2741,19 @@
       <c r="B3" s="5">
         <v>2014</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="9">
         <v>1.2222804</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="9">
         <v>0.44699749999999999</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="9">
         <v>22.9314</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="9">
         <v>2.7344233</v>
       </c>
-      <c r="G3">
+      <c r="G3" s="9">
         <v>1.18356E-2</v>
       </c>
     </row>
@@ -2477,19 +2764,19 @@
       <c r="B4" s="5">
         <v>2015</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="9">
         <v>1.2567752999999999</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="9">
         <v>0.4297879</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="9">
         <v>19.669229999999999</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="9">
         <v>2.9241755</v>
       </c>
-      <c r="G4">
+      <c r="G4" s="9">
         <v>8.4884999999999995E-3</v>
       </c>
     </row>
@@ -2500,19 +2787,19 @@
       <c r="B5">
         <v>2016</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="9">
         <v>-0.1621467</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="9">
         <v>0.44771699999999998</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="9">
         <v>22.998339999999999</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="9">
         <v>-0.36216350000000003</v>
       </c>
-      <c r="G5">
+      <c r="G5" s="9">
         <v>0.72053650000000002</v>
       </c>
     </row>
@@ -2523,19 +2810,19 @@
       <c r="B6">
         <v>2017</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="9">
         <v>-0.68085240000000002</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="9">
         <v>0.45270310000000002</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="9">
         <v>24.044969999999999</v>
       </c>
-      <c r="F6">
+      <c r="F6" s="9">
         <v>-1.5039712000000001</v>
       </c>
-      <c r="G6">
+      <c r="G6" s="9">
         <v>0.1456114</v>
       </c>
     </row>
@@ -2546,19 +2833,19 @@
       <c r="B7" s="5">
         <v>2018</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="9">
         <v>0.90447509999999998</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="9">
         <v>0.40026400000000001</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="9">
         <v>14.78186</v>
       </c>
-      <c r="F7">
+      <c r="F7" s="9">
         <v>2.2596962</v>
       </c>
-      <c r="G7">
+      <c r="G7" s="9">
         <v>3.93902E-2</v>
       </c>
     </row>
@@ -2569,19 +2856,19 @@
       <c r="B8">
         <v>2019</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="9">
         <v>-5.5265300000000003E-2</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="9">
         <v>0.44688699999999998</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="9">
         <v>22.91253</v>
       </c>
-      <c r="F8">
+      <c r="F8" s="9">
         <v>-0.1236672</v>
       </c>
-      <c r="G8">
+      <c r="G8" s="9">
         <v>0.90265720000000005</v>
       </c>
     </row>
@@ -2620,19 +2907,19 @@
       <c r="B12">
         <v>2014</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="9">
         <v>-0.14411280000000001</v>
       </c>
-      <c r="D12">
+      <c r="D12" s="9">
         <v>0.48187629999999998</v>
       </c>
-      <c r="E12">
+      <c r="E12" s="9">
         <v>339.0231</v>
       </c>
-      <c r="F12">
+      <c r="F12" s="9">
         <v>-0.299066</v>
       </c>
-      <c r="G12">
+      <c r="G12" s="9">
         <v>0.98703419999999997</v>
       </c>
     </row>
@@ -2643,19 +2930,19 @@
       <c r="B13">
         <v>2014</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="9">
         <v>-4.0036000000000004E-3</v>
       </c>
-      <c r="D13">
+      <c r="D13" s="9">
         <v>0.35429159999999998</v>
       </c>
-      <c r="E13">
+      <c r="E13" s="9">
         <v>339.00979999999998</v>
       </c>
-      <c r="F13">
+      <c r="F13" s="9">
         <v>-1.13004E-2</v>
       </c>
-      <c r="G13">
+      <c r="G13" s="9">
         <v>0.99999930000000004</v>
       </c>
     </row>
@@ -2666,19 +2953,19 @@
       <c r="B14">
         <v>2014</v>
       </c>
-      <c r="C14">
+      <c r="C14" s="9">
         <v>0.14010919999999999</v>
       </c>
-      <c r="D14">
+      <c r="D14" s="9">
         <v>0.45624120000000001</v>
       </c>
-      <c r="E14">
+      <c r="E14" s="9">
         <v>339.0102</v>
       </c>
-      <c r="F14">
+      <c r="F14" s="9">
         <v>0.3070946</v>
       </c>
-      <c r="G14">
+      <c r="G14" s="9">
         <v>0.98599550000000002</v>
       </c>
     </row>
@@ -2689,19 +2976,19 @@
       <c r="B15">
         <v>2015</v>
       </c>
-      <c r="C15">
+      <c r="C15" s="9">
         <v>-0.51327310000000004</v>
       </c>
-      <c r="D15">
+      <c r="D15" s="9">
         <v>0.37047210000000003</v>
       </c>
-      <c r="E15">
+      <c r="E15" s="9">
         <v>339.14420000000001</v>
       </c>
-      <c r="F15">
+      <c r="F15" s="9">
         <v>-1.3854568</v>
       </c>
-      <c r="G15">
+      <c r="G15" s="9">
         <v>0.42162260000000001</v>
       </c>
     </row>
@@ -2712,19 +2999,19 @@
       <c r="B16">
         <v>2015</v>
       </c>
-      <c r="C16">
+      <c r="C16" s="9">
         <v>-0.63134469999999998</v>
       </c>
-      <c r="D16">
+      <c r="D16" s="9">
         <v>0.37176949999999997</v>
       </c>
-      <c r="E16">
+      <c r="E16" s="9">
         <v>339.36900000000003</v>
       </c>
-      <c r="F16">
+      <c r="F16" s="9">
         <v>-1.6982151000000001</v>
       </c>
-      <c r="G16">
+      <c r="G16" s="9">
         <v>0.24738199999999999</v>
       </c>
     </row>
@@ -2735,19 +3022,19 @@
       <c r="B17">
         <v>2015</v>
       </c>
-      <c r="C17">
+      <c r="C17" s="9">
         <v>-0.1180716</v>
       </c>
-      <c r="D17">
+      <c r="D17" s="9">
         <v>0.3556705</v>
       </c>
-      <c r="E17">
+      <c r="E17" s="9">
         <v>339.07740000000001</v>
       </c>
-      <c r="F17">
+      <c r="F17" s="9">
         <v>-0.33196890000000001</v>
       </c>
-      <c r="G17">
+      <c r="G17" s="9">
         <v>0.98244790000000004</v>
       </c>
     </row>
@@ -2758,19 +3045,19 @@
       <c r="B18">
         <v>2016</v>
       </c>
-      <c r="C18">
+      <c r="C18" s="9">
         <v>0.85316369999999997</v>
       </c>
-      <c r="D18">
+      <c r="D18" s="9">
         <v>0.50279359999999995</v>
       </c>
-      <c r="E18">
+      <c r="E18" s="9">
         <v>339.36110000000002</v>
       </c>
-      <c r="F18">
+      <c r="F18" s="9">
         <v>1.6968468000000001</v>
       </c>
-      <c r="G18">
+      <c r="G18" s="9">
         <v>0.2480241</v>
       </c>
     </row>
@@ -2781,19 +3068,19 @@
       <c r="B19" s="5">
         <v>2016</v>
       </c>
-      <c r="C19">
+      <c r="C19" s="9">
         <v>1.3449034</v>
       </c>
-      <c r="D19">
+      <c r="D19" s="9">
         <v>0.37400499999999998</v>
       </c>
-      <c r="E19">
+      <c r="E19" s="9">
         <v>339.8485</v>
       </c>
-      <c r="F19">
+      <c r="F19" s="9">
         <v>3.5959500000000002</v>
       </c>
-      <c r="G19">
+      <c r="G19" s="9">
         <v>1.1129E-3</v>
       </c>
     </row>
@@ -2804,19 +3091,19 @@
       <c r="B20">
         <v>2016</v>
       </c>
-      <c r="C20">
+      <c r="C20" s="9">
         <v>0.4917397</v>
       </c>
-      <c r="D20">
+      <c r="D20" s="9">
         <v>0.449959</v>
       </c>
-      <c r="E20">
+      <c r="E20" s="9">
         <v>339.33429999999998</v>
       </c>
-      <c r="F20">
+      <c r="F20" s="9">
         <v>1.0928545000000001</v>
       </c>
-      <c r="G20">
+      <c r="G20" s="9">
         <v>0.61928910000000004</v>
       </c>
     </row>
@@ -2827,19 +3114,19 @@
       <c r="B21">
         <v>2017</v>
       </c>
-      <c r="C21">
+      <c r="C21" s="9">
         <v>-0.3332079</v>
       </c>
-      <c r="D21">
+      <c r="D21" s="9">
         <v>0.36237350000000002</v>
       </c>
-      <c r="E21">
+      <c r="E21" s="9">
         <v>339.00279999999998</v>
       </c>
-      <c r="F21">
+      <c r="F21" s="9">
         <v>-0.91951510000000003</v>
       </c>
-      <c r="G21">
+      <c r="G21" s="9">
         <v>0.73598379999999997</v>
       </c>
     </row>
@@ -2850,19 +3137,19 @@
       <c r="B22">
         <v>2017</v>
       </c>
-      <c r="C22">
+      <c r="C22" s="9">
         <v>0.27118130000000001</v>
       </c>
-      <c r="D22">
+      <c r="D22" s="9">
         <v>0.48515629999999998</v>
       </c>
-      <c r="E22">
+      <c r="E22" s="9">
         <v>341.02960000000002</v>
       </c>
-      <c r="F22">
+      <c r="F22" s="9">
         <v>0.55895649999999997</v>
       </c>
-      <c r="G22">
+      <c r="G22" s="9">
         <v>0.9240756</v>
       </c>
     </row>
@@ -2873,19 +3160,19 @@
       <c r="B23">
         <v>2017</v>
       </c>
-      <c r="C23">
+      <c r="C23" s="9">
         <v>0.60438919999999996</v>
       </c>
-      <c r="D23">
+      <c r="D23" s="9">
         <v>0.51144299999999998</v>
       </c>
-      <c r="E23">
+      <c r="E23" s="9">
         <v>340.82220000000001</v>
       </c>
-      <c r="F23">
+      <c r="F23" s="9">
         <v>1.1817332</v>
       </c>
-      <c r="G23">
+      <c r="G23" s="9">
         <v>0.55778519999999998</v>
       </c>
     </row>
@@ -2896,19 +3183,19 @@
       <c r="B24">
         <v>2018</v>
       </c>
-      <c r="C24">
+      <c r="C24" s="9">
         <v>9.8819199999999996E-2</v>
       </c>
-      <c r="D24">
+      <c r="D24" s="9">
         <v>0.31917450000000003</v>
       </c>
-      <c r="E24">
+      <c r="E24" s="9">
         <v>339.02879999999999</v>
       </c>
-      <c r="F24">
+      <c r="F24" s="9">
         <v>0.30960860000000001</v>
       </c>
-      <c r="G24">
+      <c r="G24" s="9">
         <v>0.98565970000000003</v>
       </c>
     </row>
@@ -2919,19 +3206,19 @@
       <c r="B25">
         <v>2018</v>
       </c>
-      <c r="C25">
+      <c r="C25" s="9">
         <v>0.50190239999999997</v>
       </c>
-      <c r="D25">
+      <c r="D25" s="9">
         <v>0.29827330000000002</v>
       </c>
-      <c r="E25">
+      <c r="E25" s="9">
         <v>339.40559999999999</v>
       </c>
-      <c r="F25">
+      <c r="F25" s="9">
         <v>1.6826928999999999</v>
       </c>
-      <c r="G25">
+      <c r="G25" s="9">
         <v>0.25473109999999999</v>
       </c>
     </row>
@@ -2942,19 +3229,19 @@
       <c r="B26">
         <v>2018</v>
       </c>
-      <c r="C26">
+      <c r="C26" s="9">
         <v>0.40308319999999997</v>
       </c>
-      <c r="D26">
+      <c r="D26" s="9">
         <v>0.32376319999999997</v>
       </c>
-      <c r="E26">
+      <c r="E26" s="9">
         <v>339.18759999999997</v>
       </c>
-      <c r="F26">
+      <c r="F26" s="9">
         <v>1.2449939999999999</v>
       </c>
-      <c r="G26">
+      <c r="G26" s="9">
         <v>0.51440010000000003</v>
       </c>
     </row>
@@ -2965,19 +3252,19 @@
       <c r="B27">
         <v>2019</v>
       </c>
-      <c r="C27">
+      <c r="C27" s="9">
         <v>0.59583050000000004</v>
       </c>
-      <c r="D27">
+      <c r="D27" s="9">
         <v>0.39688129999999999</v>
       </c>
-      <c r="E27">
+      <c r="E27" s="9">
         <v>339.0027</v>
       </c>
-      <c r="F27">
+      <c r="F27" s="9">
         <v>1.5012812</v>
       </c>
-      <c r="G27">
+      <c r="G27" s="9">
         <v>0.35101870000000002</v>
       </c>
     </row>
@@ -2988,19 +3275,19 @@
       <c r="B28">
         <v>2019</v>
       </c>
-      <c r="C28">
+      <c r="C28" s="9">
         <v>0.43950919999999999</v>
       </c>
-      <c r="D28">
+      <c r="D28" s="9">
         <v>0.39683479999999999</v>
       </c>
-      <c r="E28">
+      <c r="E28" s="9">
         <v>339.00290000000001</v>
       </c>
-      <c r="F28">
+      <c r="F28" s="9">
         <v>1.1075368999999999</v>
       </c>
-      <c r="G28">
+      <c r="G28" s="9">
         <v>0.60913689999999998</v>
       </c>
     </row>
@@ -3011,19 +3298,19 @@
       <c r="B29">
         <v>2019</v>
       </c>
-      <c r="C29">
+      <c r="C29" s="9">
         <v>-0.15632119999999999</v>
       </c>
-      <c r="D29">
+      <c r="D29" s="9">
         <v>0.39689150000000001</v>
       </c>
-      <c r="E29">
+      <c r="E29" s="9">
         <v>339.00330000000002</v>
       </c>
-      <c r="F29">
+      <c r="F29" s="9">
         <v>-0.39386389999999999</v>
       </c>
-      <c r="G29">
+      <c r="G29" s="9">
         <v>0.97132750000000001</v>
       </c>
     </row>
@@ -3052,12 +3339,13 @@
   <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="D6" sqref="D6:D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="27.85546875" customWidth="1"/>
+    <col min="5" max="5" width="22.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -3100,16 +3388,16 @@
       <c r="A6" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="9">
         <v>34.947600000000001</v>
       </c>
       <c r="C6">
         <v>1</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="9">
         <v>75.05</v>
       </c>
-      <c r="E6" s="6">
+      <c r="E6" s="9">
         <v>9.3340000000000001E-8</v>
       </c>
       <c r="F6" t="s">
@@ -3120,16 +3408,16 @@
       <c r="A7" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="9">
         <v>5.6532999999999998</v>
       </c>
       <c r="C7">
         <v>1</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="9">
         <v>40.76</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="9">
         <v>2.2197000000000001E-2</v>
       </c>
       <c r="F7" t="s">
@@ -3140,16 +3428,16 @@
       <c r="A8" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="9">
         <v>5.5955000000000004</v>
       </c>
       <c r="C8">
         <v>5</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="9">
         <v>316.69</v>
       </c>
-      <c r="E8" s="6">
+      <c r="E8" s="9">
         <v>5.8709999999999999E-5</v>
       </c>
       <c r="F8" t="s">
@@ -3160,16 +3448,16 @@
       <c r="A9" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="9">
         <v>3.0185</v>
       </c>
       <c r="C9">
         <v>2</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="9">
         <v>316.18</v>
       </c>
-      <c r="E9">
+      <c r="E9" s="9">
         <v>5.0283000000000001E-2</v>
       </c>
       <c r="F9" t="s">
@@ -3180,16 +3468,16 @@
       <c r="A10" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="9">
         <v>3.2837999999999998</v>
       </c>
       <c r="C10">
         <v>5</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="9">
         <v>316.91000000000003</v>
       </c>
-      <c r="E10">
+      <c r="E10" s="9">
         <v>6.6109999999999997E-3</v>
       </c>
       <c r="F10" t="s">
@@ -3200,16 +3488,16 @@
       <c r="A11" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="9">
         <v>2.5859999999999999</v>
       </c>
       <c r="C11">
         <v>10</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="9">
         <v>316.64999999999998</v>
       </c>
-      <c r="E11">
+      <c r="E11" s="9">
         <v>5.0340000000000003E-3</v>
       </c>
       <c r="F11" t="s">
@@ -3220,16 +3508,16 @@
       <c r="A12" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="B12">
+      <c r="B12" s="9">
         <v>0.23130000000000001</v>
       </c>
       <c r="C12">
         <v>2</v>
       </c>
-      <c r="D12">
+      <c r="D12" s="9">
         <v>316.81</v>
       </c>
-      <c r="E12">
+      <c r="E12" s="9">
         <v>0.79363799999999995</v>
       </c>
     </row>
@@ -3252,13 +3540,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0FB4343-2B3A-4546-8374-BA8176CE4411}">
   <dimension ref="A1:K31"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11:G30"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13:G30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="27.7109375" customWidth="1"/>
+    <col min="3" max="3" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.5703125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="16.5703125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3297,19 +3590,19 @@
       <c r="B3" s="5">
         <v>2014</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="9">
         <v>-1.4474119999999999</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="9">
         <v>0.5115866</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="9">
         <v>29.38242</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="9">
         <v>-2.8292619999999999</v>
       </c>
-      <c r="G3">
+      <c r="G3" s="9">
         <v>8.3254000000000002E-3</v>
       </c>
     </row>
@@ -3320,19 +3613,19 @@
       <c r="B4" s="5">
         <v>2015</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="9">
         <v>-1.2672829999999999</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="9">
         <v>0.51033360000000005</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="9">
         <v>29.044219999999999</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="9">
         <v>-2.483244</v>
       </c>
-      <c r="G4">
+      <c r="G4" s="9">
         <v>1.9037800000000001E-2</v>
       </c>
     </row>
@@ -3343,19 +3636,19 @@
       <c r="B5" s="5">
         <v>2016</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="9">
         <v>-1.895969</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="9">
         <v>0.51758470000000001</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="9">
         <v>30.609030000000001</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="9">
         <v>-3.6631079999999998</v>
       </c>
-      <c r="G5">
+      <c r="G5" s="9">
         <v>9.3499999999999996E-4</v>
       </c>
     </row>
@@ -3366,19 +3659,19 @@
       <c r="B6" s="5">
         <v>2017</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="9">
         <v>-2.2018080000000002</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="9">
         <v>0.50697809999999999</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="9">
         <v>28.361129999999999</v>
       </c>
-      <c r="F6">
+      <c r="F6" s="9">
         <v>-4.3430049999999998</v>
       </c>
-      <c r="G6">
+      <c r="G6" s="9">
         <v>1.628E-4</v>
       </c>
     </row>
@@ -3389,19 +3682,19 @@
       <c r="B7">
         <v>2018</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="9">
         <v>-0.74929800000000002</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="9">
         <v>0.4407895</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="9">
         <v>16.356110000000001</v>
       </c>
-      <c r="F7">
+      <c r="F7" s="9">
         <v>-1.6999</v>
       </c>
-      <c r="G7">
+      <c r="G7" s="9">
         <v>0.1080846</v>
       </c>
     </row>
@@ -3412,19 +3705,19 @@
       <c r="B8" s="5">
         <v>2019</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="9">
         <v>-2.4141530000000002</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="9">
         <v>0.49700240000000001</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="9">
         <v>26.359929999999999</v>
       </c>
-      <c r="F8">
+      <c r="F8" s="9">
         <v>-4.8574289999999998</v>
       </c>
-      <c r="G8">
+      <c r="G8" s="9">
         <v>4.7299999999999998E-5</v>
       </c>
     </row>
@@ -3463,19 +3756,19 @@
       <c r="B13">
         <v>2014</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="9">
         <v>-0.72276910000000005</v>
       </c>
-      <c r="D13">
+      <c r="D13" s="9">
         <v>0.60733479999999995</v>
       </c>
-      <c r="E13">
+      <c r="E13" s="9">
         <v>316.06720000000001</v>
       </c>
-      <c r="F13">
+      <c r="F13" s="9">
         <v>-1.1900671</v>
       </c>
-      <c r="G13">
+      <c r="G13" s="9">
         <v>0.55215040000000004</v>
       </c>
     </row>
@@ -3486,19 +3779,19 @@
       <c r="B14" s="5">
         <v>2014</v>
       </c>
-      <c r="C14">
+      <c r="C14" s="9">
         <v>-1.3218253</v>
       </c>
-      <c r="D14">
+      <c r="D14" s="9">
         <v>0.44545249999999997</v>
       </c>
-      <c r="E14">
+      <c r="E14" s="9">
         <v>316.6395</v>
       </c>
-      <c r="F14">
+      <c r="F14" s="9">
         <v>-2.9673764</v>
       </c>
-      <c r="G14">
+      <c r="G14" s="9">
         <v>9.6656999999999993E-3</v>
       </c>
     </row>
@@ -3509,19 +3802,19 @@
       <c r="B15">
         <v>2014</v>
       </c>
-      <c r="C15">
+      <c r="C15" s="9">
         <v>-0.59905620000000004</v>
       </c>
-      <c r="D15">
+      <c r="D15" s="9">
         <v>0.55742959999999997</v>
       </c>
-      <c r="E15">
+      <c r="E15" s="9">
         <v>316.33370000000002</v>
       </c>
-      <c r="F15">
+      <c r="F15" s="9">
         <v>-1.0746758999999999</v>
       </c>
-      <c r="G15">
+      <c r="G15" s="9">
         <v>0.63192060000000005</v>
       </c>
     </row>
@@ -3532,19 +3825,19 @@
       <c r="B16" s="5">
         <v>2015</v>
       </c>
-      <c r="C16">
+      <c r="C16" s="9">
         <v>-1.9405540999999999</v>
       </c>
-      <c r="D16">
+      <c r="D16" s="9">
         <v>0.47983680000000001</v>
       </c>
-      <c r="E16">
+      <c r="E16" s="9">
         <v>316.67360000000002</v>
       </c>
-      <c r="F16">
+      <c r="F16" s="9">
         <v>-4.0441962</v>
       </c>
-      <c r="G16">
+      <c r="G16" s="9">
         <v>1.9799999999999999E-4</v>
       </c>
     </row>
@@ -3555,19 +3848,19 @@
       <c r="B17" s="5">
         <v>2015</v>
       </c>
-      <c r="C17">
+      <c r="C17" s="9">
         <v>-1.7328106999999999</v>
       </c>
-      <c r="D17">
+      <c r="D17" s="9">
         <v>0.4958284</v>
       </c>
-      <c r="E17">
+      <c r="E17" s="9">
         <v>316.54610000000002</v>
       </c>
-      <c r="F17">
+      <c r="F17" s="9">
         <v>-3.4947794000000001</v>
       </c>
-      <c r="G17">
+      <c r="G17" s="9">
         <v>1.6255E-3</v>
       </c>
     </row>
@@ -3578,19 +3871,19 @@
       <c r="B18">
         <v>2015</v>
       </c>
-      <c r="C18">
+      <c r="C18" s="9">
         <v>0.20774339999999999</v>
       </c>
-      <c r="D18">
+      <c r="D18" s="9">
         <v>0.44811509999999999</v>
       </c>
-      <c r="E18">
+      <c r="E18" s="9">
         <v>316.31490000000002</v>
       </c>
-      <c r="F18">
+      <c r="F18" s="9">
         <v>0.4635938</v>
       </c>
-      <c r="G18">
+      <c r="G18" s="9">
         <v>0.95459910000000003</v>
       </c>
     </row>
@@ -3601,19 +3894,19 @@
       <c r="B19">
         <v>2016</v>
       </c>
-      <c r="C19">
+      <c r="C19" s="9">
         <v>-0.42381619999999998</v>
       </c>
-      <c r="D19">
+      <c r="D19" s="9">
         <v>0.6374609</v>
       </c>
-      <c r="E19">
+      <c r="E19" s="9">
         <v>316.61239999999998</v>
       </c>
-      <c r="F19">
+      <c r="F19" s="9">
         <v>-0.66485039999999995</v>
       </c>
-      <c r="G19">
+      <c r="G19" s="9">
         <v>0.87990690000000005</v>
       </c>
     </row>
@@ -3624,19 +3917,19 @@
       <c r="B20">
         <v>2016</v>
       </c>
-      <c r="C20">
+      <c r="C20" s="9">
         <v>0.94320850000000001</v>
       </c>
-      <c r="D20">
+      <c r="D20" s="9">
         <v>0.475887</v>
       </c>
-      <c r="E20">
+      <c r="E20" s="9">
         <v>317.18759999999997</v>
       </c>
-      <c r="F20">
+      <c r="F20" s="9">
         <v>1.9820009000000001</v>
       </c>
-      <c r="G20">
+      <c r="G20" s="9">
         <v>0.138128</v>
       </c>
       <c r="K20" s="2"/>
@@ -3648,19 +3941,19 @@
       <c r="B21" s="5">
         <v>2016</v>
       </c>
-      <c r="C21">
+      <c r="C21" s="9">
         <v>1.3670247</v>
       </c>
-      <c r="D21">
+      <c r="D21" s="9">
         <v>0.55660719999999997</v>
       </c>
-      <c r="E21">
+      <c r="E21" s="9">
         <v>316.66590000000002</v>
       </c>
-      <c r="F21">
+      <c r="F21" s="9">
         <v>2.4559953000000001</v>
       </c>
-      <c r="G21">
+      <c r="G21" s="9">
         <v>4.3123500000000002E-2</v>
       </c>
       <c r="K21" s="2"/>
@@ -3672,19 +3965,19 @@
       <c r="B22">
         <v>2017</v>
       </c>
-      <c r="C22">
+      <c r="C22" s="9">
         <v>-0.46677809999999997</v>
       </c>
-      <c r="D22">
+      <c r="D22" s="9">
         <v>0.42979580000000001</v>
       </c>
-      <c r="E22">
+      <c r="E22" s="9">
         <v>316.072</v>
       </c>
-      <c r="F22">
+      <c r="F22" s="9">
         <v>-1.0860462</v>
       </c>
-      <c r="G22">
+      <c r="G22" s="9">
         <v>0.62408019999999997</v>
       </c>
       <c r="K22" s="2"/>
@@ -3696,19 +3989,19 @@
       <c r="B23">
         <v>2017</v>
       </c>
-      <c r="C23">
+      <c r="C23" s="9">
         <v>-0.27691179999999999</v>
       </c>
-      <c r="D23">
+      <c r="D23" s="9">
         <v>0.56645319999999999</v>
       </c>
-      <c r="E23">
+      <c r="E23" s="9">
         <v>318.87029999999999</v>
       </c>
-      <c r="F23">
+      <c r="F23" s="9">
         <v>-0.48885200000000001</v>
       </c>
-      <c r="G23">
+      <c r="G23" s="9">
         <v>0.94738469999999997</v>
       </c>
       <c r="K23" s="2"/>
@@ -3720,19 +4013,19 @@
       <c r="B24">
         <v>2017</v>
       </c>
-      <c r="C24">
+      <c r="C24" s="9">
         <v>0.18986639999999999</v>
       </c>
-      <c r="D24">
+      <c r="D24" s="9">
         <v>0.60371419999999998</v>
       </c>
-      <c r="E24">
+      <c r="E24" s="9">
         <v>319.0883</v>
       </c>
-      <c r="F24">
+      <c r="F24" s="9">
         <v>0.31449709999999997</v>
       </c>
-      <c r="G24">
+      <c r="G24" s="9">
         <v>0.98499460000000005</v>
       </c>
       <c r="K24" s="2"/>
@@ -3744,19 +4037,19 @@
       <c r="B25" s="5">
         <v>2018</v>
       </c>
-      <c r="C25">
+      <c r="C25" s="9">
         <v>-1.0111458</v>
       </c>
-      <c r="D25">
+      <c r="D25" s="9">
         <v>0.37454340000000003</v>
       </c>
-      <c r="E25">
+      <c r="E25" s="9">
         <v>316.09809999999999</v>
       </c>
-      <c r="F25">
+      <c r="F25" s="9">
         <v>-2.6996761</v>
       </c>
-      <c r="G25">
+      <c r="G25" s="9">
         <v>2.1782599999999999E-2</v>
       </c>
       <c r="K25" s="2"/>
@@ -3768,19 +4061,19 @@
       <c r="B26">
         <v>2018</v>
       </c>
-      <c r="C26">
+      <c r="C26" s="9">
         <v>-0.7309137</v>
       </c>
-      <c r="D26">
+      <c r="D26" s="9">
         <v>0.35062149999999997</v>
       </c>
-      <c r="E26">
+      <c r="E26" s="9">
         <v>316.76979999999998</v>
       </c>
-      <c r="F26">
+      <c r="F26" s="9">
         <v>-2.0846233999999999</v>
       </c>
-      <c r="G26">
+      <c r="G26" s="9">
         <v>0.10945680000000001</v>
       </c>
       <c r="K26" s="2"/>
@@ -3792,19 +4085,19 @@
       <c r="B27">
         <v>2018</v>
       </c>
-      <c r="C27">
+      <c r="C27" s="9">
         <v>0.28023209999999998</v>
       </c>
-      <c r="D27">
+      <c r="D27" s="9">
         <v>0.37744290000000003</v>
       </c>
-      <c r="E27">
+      <c r="E27" s="9">
         <v>316.26839999999999</v>
       </c>
-      <c r="F27">
+      <c r="F27" s="9">
         <v>0.74244900000000003</v>
       </c>
-      <c r="G27">
+      <c r="G27" s="9">
         <v>0.84110260000000003</v>
       </c>
       <c r="K27" s="2"/>
@@ -3816,19 +4109,19 @@
       <c r="B28">
         <v>2019</v>
       </c>
-      <c r="C28">
+      <c r="C28" s="9">
         <v>-0.34437250000000003</v>
       </c>
-      <c r="D28">
+      <c r="D28" s="9">
         <v>0.4626575</v>
       </c>
-      <c r="E28">
+      <c r="E28" s="9">
         <v>316.00299999999999</v>
       </c>
-      <c r="F28">
+      <c r="F28" s="9">
         <v>-0.74433559999999999</v>
       </c>
-      <c r="G28">
+      <c r="G28" s="9">
         <v>0.84009730000000005</v>
       </c>
       <c r="K28" s="2"/>
@@ -3840,19 +4133,19 @@
       <c r="B29">
         <v>2019</v>
       </c>
-      <c r="C29">
+      <c r="C29" s="9">
         <v>-0.78888080000000005</v>
       </c>
-      <c r="D29">
+      <c r="D29" s="9">
         <v>0.46261140000000001</v>
       </c>
-      <c r="E29">
+      <c r="E29" s="9">
         <v>316.00470000000001</v>
       </c>
-      <c r="F29">
+      <c r="F29" s="9">
         <v>-1.7052776000000001</v>
       </c>
-      <c r="G29">
+      <c r="G29" s="9">
         <v>0.2442541</v>
       </c>
       <c r="K29" s="2"/>
@@ -3864,19 +4157,19 @@
       <c r="B30">
         <v>2019</v>
       </c>
-      <c r="C30">
+      <c r="C30" s="9">
         <v>-0.44450840000000003</v>
       </c>
-      <c r="D30">
+      <c r="D30" s="9">
         <v>0.46266679999999999</v>
       </c>
-      <c r="E30">
+      <c r="E30" s="9">
         <v>316.00470000000001</v>
       </c>
-      <c r="F30">
+      <c r="F30" s="9">
         <v>-0.96075279999999996</v>
       </c>
-      <c r="G30">
+      <c r="G30" s="9">
         <v>0.70910740000000005</v>
       </c>
       <c r="K30" s="2"/>
@@ -3904,7 +4197,7 @@
   <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:XFD5"/>
+      <selection activeCell="C6" sqref="C6:C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3952,16 +4245,16 @@
       <c r="A6" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="9">
         <v>94.525199999999998</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="10">
         <v>1</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="9">
         <v>10.55</v>
       </c>
-      <c r="E6" s="6">
+      <c r="E6" s="9">
         <v>1.356E-6</v>
       </c>
       <c r="F6" t="s">
@@ -3972,16 +4265,16 @@
       <c r="A7" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="9">
         <v>9.7042999999999999</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="10">
         <v>1</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="9">
         <v>9.0500000000000007</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="9">
         <v>1.2333E-2</v>
       </c>
       <c r="F7" t="s">
@@ -3992,16 +4285,16 @@
       <c r="A8" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="9">
         <v>2.9376000000000002</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="10">
         <v>5</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="9">
         <v>329.04</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="9">
         <v>1.3072E-2</v>
       </c>
       <c r="F8" t="s">
@@ -4012,16 +4305,16 @@
       <c r="A9" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="9">
         <v>3.2650000000000001</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="10">
         <v>2</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="9">
         <v>329.01</v>
       </c>
-      <c r="E9">
+      <c r="E9" s="9">
         <v>3.9437E-2</v>
       </c>
       <c r="F9" t="s">
@@ -4032,16 +4325,16 @@
       <c r="A10" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="9">
         <v>6.6181000000000001</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="10">
         <v>5</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="9">
         <v>329.06</v>
       </c>
-      <c r="E10" s="6">
+      <c r="E10" s="9">
         <v>6.8959999999999997E-6</v>
       </c>
       <c r="F10" t="s">
@@ -4052,16 +4345,16 @@
       <c r="A11" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="9">
         <v>1.6382000000000001</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="10">
         <v>10</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="9">
         <v>329.05</v>
       </c>
-      <c r="E11">
+      <c r="E11" s="9">
         <v>9.4579999999999997E-2</v>
       </c>
       <c r="F11" t="s">
@@ -4072,16 +4365,16 @@
       <c r="A12" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="B12">
+      <c r="B12" s="9">
         <v>6.2704000000000004</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="10">
         <v>2</v>
       </c>
-      <c r="D12">
+      <c r="D12" s="9">
         <v>329.06</v>
       </c>
-      <c r="E12">
+      <c r="E12" s="9">
         <v>2.1250000000000002E-3</v>
       </c>
       <c r="F12" t="s">
@@ -4104,466 +4397,199 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{608A0460-4DAE-480E-BE49-2A986203EA97}">
-  <dimension ref="A1:G23"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{581420B1-334D-4801-9E0F-AB9FD07C8D35}">
+  <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A16" sqref="A16:G23"/>
+      <selection activeCell="D6" sqref="D6:E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.5703125" customWidth="1"/>
-    <col min="2" max="2" width="16.28515625" customWidth="1"/>
-    <col min="12" max="12" width="22.42578125" customWidth="1"/>
-    <col min="13" max="13" width="14.42578125" customWidth="1"/>
+    <col min="1" max="1" width="27.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>58</v>
-      </c>
-      <c r="B2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C2" t="s">
-        <v>64</v>
-      </c>
-      <c r="D2" t="s">
-        <v>65</v>
-      </c>
-      <c r="E2" t="s">
-        <v>30</v>
-      </c>
-      <c r="F2" t="s">
-        <v>66</v>
-      </c>
-      <c r="G2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="B3" s="5">
-        <v>2014</v>
-      </c>
-      <c r="C3">
-        <v>3.6538819999999999</v>
-      </c>
-      <c r="D3">
-        <v>1.0993759999999999</v>
-      </c>
-      <c r="E3">
-        <v>8.5289640000000002</v>
-      </c>
-      <c r="F3">
-        <v>3.3235980000000001</v>
-      </c>
-      <c r="G3">
-        <v>9.5791999999999995E-3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="B4" s="5">
-        <v>2015</v>
-      </c>
-      <c r="C4">
-        <v>3.6646580000000002</v>
-      </c>
-      <c r="D4">
-        <v>1.0904290000000001</v>
-      </c>
-      <c r="E4">
-        <v>8.2551600000000001</v>
-      </c>
-      <c r="F4">
-        <v>3.3607480000000001</v>
-      </c>
-      <c r="G4">
-        <v>9.4801E-3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>61</v>
-      </c>
-      <c r="B5">
-        <v>2016</v>
-      </c>
-      <c r="C5">
-        <v>2.3328340000000001</v>
-      </c>
-      <c r="D5">
-        <v>1.1052040000000001</v>
-      </c>
-      <c r="E5">
-        <v>8.7099390000000003</v>
-      </c>
-      <c r="F5">
-        <v>2.110773</v>
-      </c>
-      <c r="G5">
-        <v>6.5000500000000003E-2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>61</v>
-      </c>
-      <c r="B6">
-        <v>2017</v>
+        <v>57</v>
+      </c>
+      <c r="B1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="1"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="2"/>
+      <c r="B5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" t="s">
+        <v>44</v>
+      </c>
+      <c r="E5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B6" s="9">
+        <v>71.600700000000003</v>
       </c>
       <c r="C6">
-        <v>1.2274240000000001</v>
-      </c>
-      <c r="D6">
-        <v>1.102522</v>
-      </c>
-      <c r="E6">
-        <v>8.6264389999999995</v>
-      </c>
-      <c r="F6">
-        <v>1.1132880000000001</v>
-      </c>
-      <c r="G6">
-        <v>0.29564259999999998</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="B7" s="5">
-        <v>2018</v>
+        <v>1</v>
+      </c>
+      <c r="D6" s="9">
+        <v>61.19</v>
+      </c>
+      <c r="E6" s="9">
+        <v>6.9260000000000002E-12</v>
+      </c>
+      <c r="F6" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B7" s="9">
+        <v>8.2349999999999994</v>
       </c>
       <c r="C7">
-        <v>3.1665100000000002</v>
-      </c>
-      <c r="D7">
-        <v>1.0763849999999999</v>
-      </c>
-      <c r="E7">
-        <v>7.8378379999999996</v>
-      </c>
-      <c r="F7">
-        <v>2.9418000000000002</v>
-      </c>
-      <c r="G7">
-        <v>1.90828E-2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="B8" s="5">
-        <v>2019</v>
+        <v>1</v>
+      </c>
+      <c r="D7" s="9">
+        <v>30.54</v>
+      </c>
+      <c r="E7" s="9">
+        <v>7.3921000000000004E-3</v>
+      </c>
+      <c r="F7" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B8" s="9">
+        <v>17.22</v>
       </c>
       <c r="C8">
-        <v>2.5615809999999999</v>
-      </c>
-      <c r="D8">
-        <v>1.099496</v>
-      </c>
-      <c r="E8">
-        <v>8.532724</v>
-      </c>
-      <c r="F8">
-        <v>2.329777</v>
-      </c>
-      <c r="G8">
-        <v>4.6254000000000003E-2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>58</v>
-      </c>
-      <c r="B11" t="s">
-        <v>68</v>
-      </c>
-      <c r="C11" t="s">
-        <v>64</v>
-      </c>
-      <c r="D11" t="s">
-        <v>65</v>
-      </c>
-      <c r="E11" t="s">
-        <v>30</v>
+        <v>5</v>
+      </c>
+      <c r="D8" s="9">
+        <v>333.48</v>
+      </c>
+      <c r="E8" s="9">
+        <v>3.6820000000000003E-15</v>
+      </c>
+      <c r="F8" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B9" s="9">
+        <v>1.7024999999999999</v>
+      </c>
+      <c r="C9">
+        <v>2</v>
+      </c>
+      <c r="D9" s="9">
+        <v>333.1</v>
+      </c>
+      <c r="E9" s="9">
+        <v>0.18380650000000001</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B10" s="9">
+        <v>4.9337</v>
+      </c>
+      <c r="C10">
+        <v>5</v>
+      </c>
+      <c r="D10" s="9">
+        <v>333.51</v>
+      </c>
+      <c r="E10" s="9">
+        <v>2.264E-4</v>
+      </c>
+      <c r="F10" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B11" s="9">
+        <v>4.6285999999999996</v>
+      </c>
+      <c r="C11">
+        <v>10</v>
+      </c>
+      <c r="D11" s="9">
+        <v>333.38</v>
+      </c>
+      <c r="E11" s="9">
+        <v>3.4939999999999999E-6</v>
       </c>
       <c r="F11" t="s">
-        <v>66</v>
-      </c>
-      <c r="G11" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>69</v>
+        <v>46</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B12" s="9">
+        <v>0.49869999999999998</v>
       </c>
       <c r="C12">
-        <v>2.5899770000000002</v>
-      </c>
-      <c r="D12">
-        <v>1.0633900000000001</v>
-      </c>
-      <c r="E12">
-        <v>7.4673660000000002</v>
-      </c>
-      <c r="F12">
-        <v>2.435584</v>
-      </c>
-      <c r="G12">
-        <v>4.2934E-2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="C13">
-        <v>3.4945710000000001</v>
-      </c>
-      <c r="D13">
-        <v>1.0718620000000001</v>
-      </c>
-      <c r="E13">
-        <v>7.7080200000000003</v>
-      </c>
-      <c r="F13">
-        <v>3.2602799999999998</v>
-      </c>
-      <c r="G13">
-        <v>1.2124299999999999E-2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>61</v>
-      </c>
-      <c r="B14" t="s">
-        <v>71</v>
-      </c>
-      <c r="C14">
-        <v>2.2188970000000001</v>
-      </c>
-      <c r="D14">
-        <v>1.064174</v>
-      </c>
-      <c r="E14">
-        <v>7.4889239999999999</v>
-      </c>
-      <c r="F14">
-        <v>2.0850870000000001</v>
-      </c>
-      <c r="G14">
-        <v>7.2922299999999995E-2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="4" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>33</v>
-      </c>
-      <c r="B17" t="s">
-        <v>29</v>
-      </c>
-      <c r="C17" t="s">
-        <v>25</v>
-      </c>
-      <c r="D17" t="s">
-        <v>26</v>
-      </c>
-      <c r="E17" t="s">
-        <v>30</v>
-      </c>
-      <c r="F17" t="s">
-        <v>27</v>
-      </c>
-      <c r="G17" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>35</v>
-      </c>
-      <c r="B18" t="s">
-        <v>31</v>
-      </c>
-      <c r="C18">
-        <v>-0.1036161</v>
-      </c>
-      <c r="D18">
-        <v>0.26980330000000002</v>
-      </c>
-      <c r="E18">
-        <v>329.00450000000001</v>
-      </c>
-      <c r="F18">
-        <v>-0.38404300000000002</v>
-      </c>
-      <c r="G18">
-        <v>0.97332129999999994</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>36</v>
-      </c>
-      <c r="B19" t="s">
-        <v>31</v>
-      </c>
-      <c r="C19">
-        <v>0.58866350000000001</v>
-      </c>
-      <c r="D19">
-        <v>0.25318770000000002</v>
-      </c>
-      <c r="E19">
-        <v>329.00630000000001</v>
-      </c>
-      <c r="F19">
-        <v>2.3250082999999999</v>
-      </c>
-      <c r="G19">
-        <v>6.07643E-2</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="B20" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="C20">
-        <v>0.69227959999999999</v>
-      </c>
-      <c r="D20">
-        <v>0.27322590000000002</v>
-      </c>
-      <c r="E20">
-        <v>329.00819999999999</v>
-      </c>
-      <c r="F20">
-        <v>2.5337261</v>
-      </c>
-      <c r="G20">
-        <v>3.4835699999999997E-2</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="B21" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="C21">
-        <v>0.80097830000000003</v>
-      </c>
-      <c r="D21">
-        <v>0.2534402</v>
-      </c>
-      <c r="E21">
-        <v>329.03910000000002</v>
-      </c>
-      <c r="F21">
-        <v>3.1604231999999999</v>
-      </c>
-      <c r="G21">
-        <v>5.1564000000000002E-3</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>36</v>
-      </c>
-      <c r="B22" t="s">
-        <v>32</v>
-      </c>
-      <c r="C22">
-        <v>0.21758350000000001</v>
-      </c>
-      <c r="D22">
-        <v>0.2365738</v>
-      </c>
-      <c r="E22">
-        <v>329.125</v>
-      </c>
-      <c r="F22">
-        <v>0.91972759999999998</v>
-      </c>
-      <c r="G22">
-        <v>0.7358711</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>37</v>
-      </c>
-      <c r="B23" t="s">
-        <v>32</v>
-      </c>
-      <c r="C23">
-        <v>-0.58339479999999999</v>
-      </c>
-      <c r="D23">
-        <v>0.263714</v>
-      </c>
-      <c r="E23">
-        <v>329.24059999999997</v>
-      </c>
-      <c r="F23">
-        <v>-2.2122255000000002</v>
-      </c>
-      <c r="G23">
-        <v>8.0641000000000004E-2</v>
+        <v>2</v>
+      </c>
+      <c r="D12" s="9">
+        <v>333.23</v>
+      </c>
+      <c r="E12" s="9">
+        <v>0.60778109999999996</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>43</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="G3:G8">
-    <cfRule type="cellIs" dxfId="4" priority="3" operator="lessThan">
-      <formula>0.06</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G12:G14">
-    <cfRule type="cellIs" dxfId="3" priority="2" operator="lessThan">
-      <formula>0.06</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G18:G23">
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="lessThan">
-      <formula>0.06</formula>
-    </cfRule>
-  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>